<commit_message>
updated the tasks directory'
</commit_message>
<xml_diff>
--- a/results/Quantitative-Results-of-Task1-Task14.xlsx
+++ b/results/Quantitative-Results-of-Task1-Task14.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Task1" sheetId="1" state="visible" r:id="rId2"/>
@@ -87,7 +87,7 @@
     <t xml:space="preserve">** Unlimited time</t>
   </si>
   <si>
-    <t xml:space="preserve">T12: Given two highlighted nodes and three named ones, which of the named nodes is connected to both highlighted nodes?</t>
+    <t xml:space="preserve">Task12: Given two highlighted nodes and three named ones, which of the named nodes is connected to both highlighted nodes?</t>
   </si>
   <si>
     <t xml:space="preserve">Task13: Given a selected node, how many nodes are within two edges' reach?</t>
@@ -305,8 +305,8 @@
   </sheetPr>
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1989,7 +1989,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2449,8 +2449,8 @@
   </sheetPr>
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2460,7 +2460,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="25" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="8.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="29" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -3207,7 +3207,7 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3945,8 +3945,8 @@
   </sheetPr>
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4439,7 +4439,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5348,7 +5348,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6260,7 +6260,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7049,7 +7049,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7850,7 +7850,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8643,7 +8643,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9437,7 +9437,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10231,7 +10231,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>